<commit_message>
Added explaination to status flags in jump command
</commit_message>
<xml_diff>
--- a/MicrocontrollerOpCodeLibrary.xlsx
+++ b/MicrocontrollerOpCodeLibrary.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UniversityNotes\MicroControllerProject\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ashri\Desktop\MyFiles\UniversityNotes\MicroControllerProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{171ED8FF-74C4-4C6D-B3E8-CD0D77E9131D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40BB3ED0-5843-49FF-AEBC-015DBF46F2C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{364A80C0-F09F-4BB5-B341-ED023A1C648D}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="90">
   <si>
     <t>ArShift</t>
   </si>
@@ -280,6 +280,30 @@
   </si>
   <si>
     <t>RIGHTout</t>
+  </si>
+  <si>
+    <t>RIGHTout, v, c, n, z, and jmp are status flags that can control under which circumstances a jump will occur: (only one should be set to 1 at a time)</t>
+  </si>
+  <si>
+    <t>RIGHTout - last value shifted right had a most significant bit of 1</t>
+  </si>
+  <si>
+    <t>c - result from ALU had a carry out</t>
+  </si>
+  <si>
+    <t>v - result from the ALU had overflow</t>
+  </si>
+  <si>
+    <t>z - result from the ALU was zero</t>
+  </si>
+  <si>
+    <t>n -  result from ALUwas negative</t>
+  </si>
+  <si>
+    <t>jmp - no condition needed</t>
+  </si>
+  <si>
+    <t>A,B,C indiacte either the program  memory or the RAM (same length different location) location</t>
   </si>
 </sst>
 </file>
@@ -440,7 +464,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -457,13 +481,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
@@ -471,10 +488,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -485,19 +498,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
@@ -509,20 +516,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -532,11 +530,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -843,7 +837,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -851,10 +845,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80BD5700-5950-4C93-B4E2-42A8A8CD9C9B}">
-  <dimension ref="A2:AX40"/>
+  <dimension ref="A2:AT30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
-      <selection activeCell="AH24" sqref="AH24"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AC27" sqref="AC27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -899,37 +893,34 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:46" x14ac:dyDescent="0.3">
-      <c r="P2" s="30" t="s">
+      <c r="P2" s="21" t="s">
         <v>73</v>
       </c>
-      <c r="R2" s="8"/>
-      <c r="S2" s="8"/>
-      <c r="V2" s="8"/>
       <c r="AJ2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="AK2" s="19" t="s">
+      <c r="AK2" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="AL2" s="19" t="s">
+      <c r="AL2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="AM2" s="19" t="s">
+      <c r="AM2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="AN2" s="19" t="s">
+      <c r="AN2" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="AO2" s="19" t="s">
+      <c r="AO2" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="AP2" s="19" t="s">
+      <c r="AP2" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="AQ2" s="19" t="s">
+      <c r="AQ2" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="AR2" s="26" t="s">
+      <c r="AR2" s="8" t="s">
         <v>23</v>
       </c>
       <c r="AS2" s="1" t="s">
@@ -937,8 +928,6 @@
       </c>
     </row>
     <row r="3" spans="1:46" x14ac:dyDescent="0.3">
-      <c r="R3" s="8"/>
-      <c r="S3" s="8"/>
       <c r="AJ3">
         <v>0</v>
       </c>
@@ -963,7 +952,7 @@
       <c r="AQ3">
         <v>0</v>
       </c>
-      <c r="AR3" s="10">
+      <c r="AR3" s="7">
         <v>0</v>
       </c>
       <c r="AS3" t="s">
@@ -971,7 +960,7 @@
       </c>
     </row>
     <row r="4" spans="1:46" x14ac:dyDescent="0.3">
-      <c r="A4" s="36" t="s">
+      <c r="A4" s="25" t="s">
         <v>74</v>
       </c>
       <c r="B4" s="3" t="s">
@@ -1022,49 +1011,49 @@
       <c r="Q4" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="R4" s="11" t="s">
+      <c r="R4" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="S4" s="16" t="s">
-        <v>0</v>
-      </c>
-      <c r="T4" s="19" t="s">
+      <c r="S4" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="T4" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="U4" s="19" t="s">
+      <c r="U4" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="V4" s="19" t="s">
+      <c r="V4" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="W4" s="19" t="s">
+      <c r="W4" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="X4" s="19" t="s">
+      <c r="X4" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="Y4" s="19" t="s">
+      <c r="Y4" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="Z4" s="19" t="s">
+      <c r="Z4" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="AA4" s="19" t="s">
+      <c r="AA4" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="AB4" s="19" t="s">
+      <c r="AB4" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="AC4" s="19" t="s">
+      <c r="AC4" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="AD4" s="19" t="s">
+      <c r="AD4" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="AE4" s="19" t="s">
+      <c r="AE4" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="AF4" s="26" t="s">
+      <c r="AF4" s="8" t="s">
         <v>23</v>
       </c>
       <c r="AG4" s="3" t="s">
@@ -1097,18 +1086,18 @@
       <c r="AQ4">
         <v>0</v>
       </c>
-      <c r="AR4" s="10">
+      <c r="AR4" s="7">
         <v>0</v>
       </c>
       <c r="AS4" t="s">
         <v>1</v>
       </c>
-      <c r="AT4" s="28" t="s">
+      <c r="AT4" s="20" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="5" spans="1:46" x14ac:dyDescent="0.3">
-      <c r="A5" s="9">
+      <c r="A5" s="6">
         <v>0</v>
       </c>
       <c r="B5" s="5">
@@ -1159,52 +1148,52 @@
       <c r="Q5" s="5">
         <v>0</v>
       </c>
-      <c r="R5" s="31">
-        <v>1</v>
-      </c>
-      <c r="S5" s="32">
-        <v>0</v>
-      </c>
-      <c r="T5" s="32">
-        <v>0</v>
-      </c>
-      <c r="U5" s="32">
-        <v>0</v>
-      </c>
-      <c r="V5" s="32">
-        <v>0</v>
-      </c>
-      <c r="W5" s="32">
-        <v>0</v>
-      </c>
-      <c r="X5" s="32">
-        <v>0</v>
-      </c>
-      <c r="Y5" s="32">
-        <v>0</v>
-      </c>
-      <c r="Z5" s="32">
-        <v>0</v>
-      </c>
-      <c r="AA5" s="32">
-        <v>0</v>
-      </c>
-      <c r="AB5" s="32">
-        <v>0</v>
-      </c>
-      <c r="AC5" s="32">
-        <v>0</v>
-      </c>
-      <c r="AD5" s="32">
-        <v>0</v>
-      </c>
-      <c r="AE5" s="32">
-        <v>0</v>
-      </c>
-      <c r="AF5" s="33">
-        <v>0</v>
-      </c>
-      <c r="AG5" s="27" t="s">
+      <c r="R5" s="15">
+        <v>1</v>
+      </c>
+      <c r="S5" s="22">
+        <v>0</v>
+      </c>
+      <c r="T5" s="22">
+        <v>0</v>
+      </c>
+      <c r="U5" s="22">
+        <v>0</v>
+      </c>
+      <c r="V5" s="22">
+        <v>0</v>
+      </c>
+      <c r="W5" s="22">
+        <v>0</v>
+      </c>
+      <c r="X5" s="22">
+        <v>0</v>
+      </c>
+      <c r="Y5" s="22">
+        <v>0</v>
+      </c>
+      <c r="Z5" s="22">
+        <v>0</v>
+      </c>
+      <c r="AA5" s="22">
+        <v>0</v>
+      </c>
+      <c r="AB5" s="22">
+        <v>0</v>
+      </c>
+      <c r="AC5" s="22">
+        <v>0</v>
+      </c>
+      <c r="AD5" s="22">
+        <v>0</v>
+      </c>
+      <c r="AE5" s="22">
+        <v>0</v>
+      </c>
+      <c r="AF5" s="23">
+        <v>0</v>
+      </c>
+      <c r="AG5" s="19" t="s">
         <v>33</v>
       </c>
       <c r="AH5" t="s">
@@ -1234,7 +1223,7 @@
       <c r="AQ5">
         <v>0</v>
       </c>
-      <c r="AR5" s="10">
+      <c r="AR5" s="7">
         <v>0</v>
       </c>
       <c r="AS5" t="s">
@@ -1245,7 +1234,7 @@
       </c>
     </row>
     <row r="6" spans="1:46" x14ac:dyDescent="0.3">
-      <c r="A6" s="9">
+      <c r="A6" s="6">
         <v>0</v>
       </c>
       <c r="B6" s="3">
@@ -1296,52 +1285,52 @@
       <c r="Q6" s="3">
         <v>0</v>
       </c>
-      <c r="R6" s="11">
-        <v>0</v>
-      </c>
-      <c r="S6" s="34">
-        <v>0</v>
-      </c>
-      <c r="T6" s="32">
-        <v>0</v>
-      </c>
-      <c r="U6" s="32">
-        <v>0</v>
-      </c>
-      <c r="V6" s="32">
-        <v>0</v>
-      </c>
-      <c r="W6" s="32">
-        <v>0</v>
-      </c>
-      <c r="X6" s="32">
-        <v>0</v>
-      </c>
-      <c r="Y6" s="32">
-        <v>0</v>
-      </c>
-      <c r="Z6" s="32">
-        <v>0</v>
-      </c>
-      <c r="AA6" s="32">
-        <v>0</v>
-      </c>
-      <c r="AB6" s="32">
-        <v>0</v>
-      </c>
-      <c r="AC6" s="32">
-        <v>0</v>
-      </c>
-      <c r="AD6" s="32">
-        <v>0</v>
-      </c>
-      <c r="AE6" s="32">
-        <v>0</v>
-      </c>
-      <c r="AF6" s="33">
-        <v>0</v>
-      </c>
-      <c r="AG6" s="20" t="s">
+      <c r="R6" s="8">
+        <v>0</v>
+      </c>
+      <c r="S6" s="24">
+        <v>0</v>
+      </c>
+      <c r="T6" s="22">
+        <v>0</v>
+      </c>
+      <c r="U6" s="22">
+        <v>0</v>
+      </c>
+      <c r="V6" s="22">
+        <v>0</v>
+      </c>
+      <c r="W6" s="22">
+        <v>0</v>
+      </c>
+      <c r="X6" s="22">
+        <v>0</v>
+      </c>
+      <c r="Y6" s="22">
+        <v>0</v>
+      </c>
+      <c r="Z6" s="22">
+        <v>0</v>
+      </c>
+      <c r="AA6" s="22">
+        <v>0</v>
+      </c>
+      <c r="AB6" s="22">
+        <v>0</v>
+      </c>
+      <c r="AC6" s="22">
+        <v>0</v>
+      </c>
+      <c r="AD6" s="22">
+        <v>0</v>
+      </c>
+      <c r="AE6" s="22">
+        <v>0</v>
+      </c>
+      <c r="AF6" s="23">
+        <v>0</v>
+      </c>
+      <c r="AG6" s="14" t="s">
         <v>33</v>
       </c>
       <c r="AH6" s="5" t="s">
@@ -1371,18 +1360,18 @@
       <c r="AQ6">
         <v>0</v>
       </c>
-      <c r="AR6" s="10">
+      <c r="AR6" s="7">
         <v>0</v>
       </c>
       <c r="AS6" t="s">
         <v>40</v>
       </c>
-      <c r="AT6" s="27" t="s">
+      <c r="AT6" s="19" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="7" spans="1:46" x14ac:dyDescent="0.3">
-      <c r="A7" s="9">
+      <c r="A7" s="6">
         <v>0</v>
       </c>
       <c r="B7" s="3">
@@ -1433,52 +1422,52 @@
       <c r="Q7" s="3">
         <v>0</v>
       </c>
-      <c r="R7" s="11">
-        <v>0</v>
-      </c>
-      <c r="S7" s="15">
-        <v>0</v>
-      </c>
-      <c r="T7" s="15">
-        <v>0</v>
-      </c>
-      <c r="U7" s="15">
-        <v>0</v>
-      </c>
-      <c r="V7" s="15">
-        <v>0</v>
-      </c>
-      <c r="W7" s="15">
-        <v>0</v>
-      </c>
-      <c r="X7" s="15">
-        <v>0</v>
-      </c>
-      <c r="Y7" s="15">
-        <v>0</v>
-      </c>
-      <c r="Z7" s="15">
-        <v>0</v>
-      </c>
-      <c r="AA7" s="15">
-        <v>0</v>
-      </c>
-      <c r="AB7" s="15">
-        <v>0</v>
-      </c>
-      <c r="AC7" s="15">
-        <v>0</v>
-      </c>
-      <c r="AD7" s="15">
-        <v>0</v>
-      </c>
-      <c r="AE7" s="15">
-        <v>0</v>
-      </c>
-      <c r="AF7" s="23">
-        <v>0</v>
-      </c>
-      <c r="AG7" s="20" t="s">
+      <c r="R7" s="8">
+        <v>0</v>
+      </c>
+      <c r="S7" s="10">
+        <v>0</v>
+      </c>
+      <c r="T7" s="10">
+        <v>0</v>
+      </c>
+      <c r="U7" s="10">
+        <v>0</v>
+      </c>
+      <c r="V7" s="10">
+        <v>0</v>
+      </c>
+      <c r="W7" s="10">
+        <v>0</v>
+      </c>
+      <c r="X7" s="10">
+        <v>0</v>
+      </c>
+      <c r="Y7" s="10">
+        <v>0</v>
+      </c>
+      <c r="Z7" s="10">
+        <v>0</v>
+      </c>
+      <c r="AA7" s="10">
+        <v>0</v>
+      </c>
+      <c r="AB7" s="10">
+        <v>0</v>
+      </c>
+      <c r="AC7" s="10">
+        <v>0</v>
+      </c>
+      <c r="AD7" s="10">
+        <v>0</v>
+      </c>
+      <c r="AE7" s="10">
+        <v>0</v>
+      </c>
+      <c r="AF7" s="16">
+        <v>0</v>
+      </c>
+      <c r="AG7" s="14" t="s">
         <v>33</v>
       </c>
       <c r="AH7" s="5" t="s">
@@ -1508,7 +1497,7 @@
       <c r="AQ7">
         <v>0</v>
       </c>
-      <c r="AR7" s="10">
+      <c r="AR7" s="7">
         <v>0</v>
       </c>
       <c r="AS7" t="s">
@@ -1519,7 +1508,7 @@
       </c>
     </row>
     <row r="8" spans="1:46" x14ac:dyDescent="0.3">
-      <c r="A8" s="9">
+      <c r="A8" s="6">
         <v>0</v>
       </c>
       <c r="B8" s="3">
@@ -1570,52 +1559,52 @@
       <c r="Q8" s="3">
         <v>0</v>
       </c>
-      <c r="R8" s="11">
-        <v>0</v>
-      </c>
-      <c r="S8" s="15">
-        <v>0</v>
-      </c>
-      <c r="T8" s="15">
-        <v>0</v>
-      </c>
-      <c r="U8" s="15">
-        <v>0</v>
-      </c>
-      <c r="V8" s="15">
-        <v>0</v>
-      </c>
-      <c r="W8" s="15">
-        <v>0</v>
-      </c>
-      <c r="X8" s="15">
-        <v>0</v>
-      </c>
-      <c r="Y8" s="15">
-        <v>0</v>
-      </c>
-      <c r="Z8" s="15">
-        <v>0</v>
-      </c>
-      <c r="AA8" s="15">
-        <v>0</v>
-      </c>
-      <c r="AB8" s="15">
-        <v>0</v>
-      </c>
-      <c r="AC8" s="15">
-        <v>0</v>
-      </c>
-      <c r="AD8" s="15">
-        <v>0</v>
-      </c>
-      <c r="AE8" s="15">
-        <v>0</v>
-      </c>
-      <c r="AF8" s="23">
-        <v>0</v>
-      </c>
-      <c r="AG8" s="20" t="s">
+      <c r="R8" s="8">
+        <v>0</v>
+      </c>
+      <c r="S8" s="10">
+        <v>0</v>
+      </c>
+      <c r="T8" s="10">
+        <v>0</v>
+      </c>
+      <c r="U8" s="10">
+        <v>0</v>
+      </c>
+      <c r="V8" s="10">
+        <v>0</v>
+      </c>
+      <c r="W8" s="10">
+        <v>0</v>
+      </c>
+      <c r="X8" s="10">
+        <v>0</v>
+      </c>
+      <c r="Y8" s="10">
+        <v>0</v>
+      </c>
+      <c r="Z8" s="10">
+        <v>0</v>
+      </c>
+      <c r="AA8" s="10">
+        <v>0</v>
+      </c>
+      <c r="AB8" s="10">
+        <v>0</v>
+      </c>
+      <c r="AC8" s="10">
+        <v>0</v>
+      </c>
+      <c r="AD8" s="10">
+        <v>0</v>
+      </c>
+      <c r="AE8" s="10">
+        <v>0</v>
+      </c>
+      <c r="AF8" s="16">
+        <v>0</v>
+      </c>
+      <c r="AG8" s="14" t="s">
         <v>33</v>
       </c>
       <c r="AH8" s="5" t="s">
@@ -1645,18 +1634,18 @@
       <c r="AQ8">
         <v>0</v>
       </c>
-      <c r="AR8" s="10">
+      <c r="AR8" s="7">
         <v>0</v>
       </c>
       <c r="AS8" t="s">
         <v>42</v>
       </c>
-      <c r="AT8" s="27" t="s">
+      <c r="AT8" s="19" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="9" spans="1:46" x14ac:dyDescent="0.3">
-      <c r="A9" s="13">
+      <c r="A9">
         <v>0</v>
       </c>
       <c r="B9" s="4">
@@ -1707,55 +1696,55 @@
       <c r="Q9" s="4">
         <v>1</v>
       </c>
-      <c r="R9" s="12">
-        <v>1</v>
-      </c>
-      <c r="S9" s="15">
-        <v>0</v>
-      </c>
-      <c r="T9" s="15">
-        <v>0</v>
-      </c>
-      <c r="U9" s="15">
-        <v>0</v>
-      </c>
-      <c r="V9" s="15">
-        <v>0</v>
-      </c>
-      <c r="W9" s="15">
-        <v>0</v>
-      </c>
-      <c r="X9" s="15">
-        <v>0</v>
-      </c>
-      <c r="Y9" s="15">
-        <v>0</v>
-      </c>
-      <c r="Z9" s="15">
-        <v>0</v>
-      </c>
-      <c r="AA9" s="15">
-        <v>0</v>
-      </c>
-      <c r="AB9" s="15">
-        <v>0</v>
-      </c>
-      <c r="AC9" s="15">
-        <v>0</v>
-      </c>
-      <c r="AD9" s="15">
-        <v>0</v>
-      </c>
-      <c r="AE9" s="15">
-        <v>0</v>
-      </c>
-      <c r="AF9" s="23">
-        <v>0</v>
-      </c>
-      <c r="AG9" s="6" t="s">
+      <c r="R9" s="9">
+        <v>1</v>
+      </c>
+      <c r="S9" s="10">
+        <v>0</v>
+      </c>
+      <c r="T9" s="10">
+        <v>0</v>
+      </c>
+      <c r="U9" s="10">
+        <v>0</v>
+      </c>
+      <c r="V9" s="10">
+        <v>0</v>
+      </c>
+      <c r="W9" s="10">
+        <v>0</v>
+      </c>
+      <c r="X9" s="10">
+        <v>0</v>
+      </c>
+      <c r="Y9" s="10">
+        <v>0</v>
+      </c>
+      <c r="Z9" s="10">
+        <v>0</v>
+      </c>
+      <c r="AA9" s="10">
+        <v>0</v>
+      </c>
+      <c r="AB9" s="10">
+        <v>0</v>
+      </c>
+      <c r="AC9" s="10">
+        <v>0</v>
+      </c>
+      <c r="AD9" s="10">
+        <v>0</v>
+      </c>
+      <c r="AE9" s="10">
+        <v>0</v>
+      </c>
+      <c r="AF9" s="16">
+        <v>0</v>
+      </c>
+      <c r="AG9" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="AH9" s="7" t="s">
+      <c r="AH9" s="4" t="s">
         <v>26</v>
       </c>
       <c r="AJ9">
@@ -1782,7 +1771,7 @@
       <c r="AQ9">
         <v>0</v>
       </c>
-      <c r="AR9" s="10">
+      <c r="AR9" s="7">
         <v>0</v>
       </c>
       <c r="AS9" t="s">
@@ -1790,7 +1779,7 @@
       </c>
     </row>
     <row r="10" spans="1:46" x14ac:dyDescent="0.3">
-      <c r="A10" s="36">
+      <c r="A10" s="25">
         <v>0</v>
       </c>
       <c r="B10" s="3">
@@ -1841,10 +1830,10 @@
       <c r="Q10" s="3">
         <v>0</v>
       </c>
-      <c r="R10" s="11">
-        <v>0</v>
-      </c>
-      <c r="S10" s="16">
+      <c r="R10" s="8">
+        <v>0</v>
+      </c>
+      <c r="S10" s="11">
         <v>0</v>
       </c>
       <c r="T10" s="1">
@@ -1883,7 +1872,7 @@
       <c r="AE10" s="1">
         <v>0</v>
       </c>
-      <c r="AF10" s="25">
+      <c r="AF10" s="18">
         <v>0</v>
       </c>
       <c r="AG10" s="3" t="s">
@@ -1914,7 +1903,7 @@
       <c r="AQ10">
         <v>0</v>
       </c>
-      <c r="AR10" s="10">
+      <c r="AR10" s="7">
         <v>0</v>
       </c>
       <c r="AS10" t="s">
@@ -1922,7 +1911,7 @@
       </c>
     </row>
     <row r="11" spans="1:46" x14ac:dyDescent="0.3">
-      <c r="A11" s="13">
+      <c r="A11">
         <v>0</v>
       </c>
       <c r="B11" s="4">
@@ -1973,52 +1962,52 @@
       <c r="Q11" s="4">
         <v>0</v>
       </c>
-      <c r="R11" s="6">
-        <v>1</v>
-      </c>
-      <c r="S11" s="17">
-        <v>0</v>
-      </c>
-      <c r="T11" s="14">
-        <v>0</v>
-      </c>
-      <c r="U11" s="14">
-        <v>0</v>
-      </c>
-      <c r="V11" s="14">
-        <v>0</v>
-      </c>
-      <c r="W11" s="14">
-        <v>1</v>
-      </c>
-      <c r="X11" s="14">
-        <v>0</v>
-      </c>
-      <c r="Y11" s="14">
-        <v>0</v>
-      </c>
-      <c r="Z11" s="14">
-        <v>0</v>
-      </c>
-      <c r="AA11" s="14">
-        <v>0</v>
-      </c>
-      <c r="AB11" s="14">
-        <v>0</v>
-      </c>
-      <c r="AC11" s="14">
-        <v>0</v>
-      </c>
-      <c r="AD11" s="14">
-        <v>0</v>
-      </c>
-      <c r="AE11" s="14">
-        <v>0</v>
-      </c>
-      <c r="AF11" s="24">
-        <v>0</v>
-      </c>
-      <c r="AG11" s="7" t="s">
+      <c r="R11" s="4">
+        <v>1</v>
+      </c>
+      <c r="S11" s="12">
+        <v>0</v>
+      </c>
+      <c r="T11" s="2">
+        <v>0</v>
+      </c>
+      <c r="U11" s="2">
+        <v>0</v>
+      </c>
+      <c r="V11" s="2">
+        <v>0</v>
+      </c>
+      <c r="W11" s="2">
+        <v>1</v>
+      </c>
+      <c r="X11" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y11" s="2">
+        <v>0</v>
+      </c>
+      <c r="Z11" s="2">
+        <v>0</v>
+      </c>
+      <c r="AA11" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB11" s="2">
+        <v>0</v>
+      </c>
+      <c r="AC11" s="2">
+        <v>0</v>
+      </c>
+      <c r="AD11" s="2">
+        <v>0</v>
+      </c>
+      <c r="AE11" s="2">
+        <v>0</v>
+      </c>
+      <c r="AF11" s="17">
+        <v>0</v>
+      </c>
+      <c r="AG11" s="4" t="s">
         <v>24</v>
       </c>
       <c r="AH11" s="2" t="s">
@@ -2048,7 +2037,7 @@
       <c r="AQ11">
         <v>0</v>
       </c>
-      <c r="AR11" s="10">
+      <c r="AR11" s="7">
         <v>1</v>
       </c>
       <c r="AS11" t="s">
@@ -2056,7 +2045,7 @@
       </c>
     </row>
     <row r="12" spans="1:46" x14ac:dyDescent="0.3">
-      <c r="A12" s="13">
+      <c r="A12">
         <v>0</v>
       </c>
       <c r="B12" s="4">
@@ -2107,52 +2096,52 @@
       <c r="Q12" s="4">
         <v>0</v>
       </c>
-      <c r="R12" s="12">
-        <v>1</v>
-      </c>
-      <c r="S12" s="18">
-        <v>0</v>
-      </c>
-      <c r="T12" s="14">
-        <v>1</v>
-      </c>
-      <c r="U12" s="14">
-        <v>0</v>
-      </c>
-      <c r="V12" s="14">
-        <v>0</v>
-      </c>
-      <c r="W12" s="14">
-        <v>0</v>
-      </c>
-      <c r="X12" s="14">
-        <v>0</v>
-      </c>
-      <c r="Y12" s="14">
-        <v>0</v>
-      </c>
-      <c r="Z12" s="14">
-        <v>0</v>
-      </c>
-      <c r="AA12" s="14">
-        <v>0</v>
-      </c>
-      <c r="AB12" s="14">
-        <v>0</v>
-      </c>
-      <c r="AC12" s="14">
-        <v>0</v>
-      </c>
-      <c r="AD12" s="14">
-        <v>0</v>
-      </c>
-      <c r="AE12" s="14">
-        <v>0</v>
-      </c>
-      <c r="AF12" s="24">
-        <v>0</v>
-      </c>
-      <c r="AG12" s="7" t="s">
+      <c r="R12" s="9">
+        <v>1</v>
+      </c>
+      <c r="S12" s="13">
+        <v>0</v>
+      </c>
+      <c r="T12" s="2">
+        <v>1</v>
+      </c>
+      <c r="U12" s="2">
+        <v>0</v>
+      </c>
+      <c r="V12" s="2">
+        <v>0</v>
+      </c>
+      <c r="W12" s="2">
+        <v>0</v>
+      </c>
+      <c r="X12" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y12" s="2">
+        <v>0</v>
+      </c>
+      <c r="Z12" s="2">
+        <v>0</v>
+      </c>
+      <c r="AA12" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB12" s="2">
+        <v>0</v>
+      </c>
+      <c r="AC12" s="2">
+        <v>0</v>
+      </c>
+      <c r="AD12" s="2">
+        <v>0</v>
+      </c>
+      <c r="AE12" s="2">
+        <v>0</v>
+      </c>
+      <c r="AF12" s="17">
+        <v>0</v>
+      </c>
+      <c r="AG12" s="4" t="s">
         <v>65</v>
       </c>
       <c r="AH12" s="2"/>
@@ -2180,7 +2169,7 @@
       <c r="AQ12">
         <v>0</v>
       </c>
-      <c r="AR12" s="10">
+      <c r="AR12" s="7">
         <v>1</v>
       </c>
       <c r="AS12" t="s">
@@ -2188,7 +2177,7 @@
       </c>
     </row>
     <row r="13" spans="1:46" x14ac:dyDescent="0.3">
-      <c r="A13" s="36">
+      <c r="A13" s="25">
         <v>0</v>
       </c>
       <c r="B13" s="3">
@@ -2239,49 +2228,49 @@
       <c r="Q13" s="3">
         <v>0</v>
       </c>
-      <c r="R13" s="26">
-        <v>1</v>
-      </c>
-      <c r="S13" s="35" t="s">
+      <c r="R13" s="8">
+        <v>1</v>
+      </c>
+      <c r="S13" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="T13" s="19">
-        <v>0</v>
-      </c>
-      <c r="U13" s="19" t="s">
+      <c r="T13" s="3">
+        <v>0</v>
+      </c>
+      <c r="U13" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="V13" s="19" t="s">
+      <c r="V13" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="W13" s="19">
-        <v>0</v>
-      </c>
-      <c r="X13" s="19" t="s">
+      <c r="W13" s="3">
+        <v>0</v>
+      </c>
+      <c r="X13" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="Y13" s="19" t="s">
+      <c r="Y13" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="Z13" s="19" t="s">
+      <c r="Z13" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="AA13" s="19">
-        <v>1</v>
-      </c>
-      <c r="AB13" s="19">
-        <v>0</v>
-      </c>
-      <c r="AC13" s="19">
-        <v>0</v>
-      </c>
-      <c r="AD13" s="19" t="s">
+      <c r="AA13" s="3">
+        <v>1</v>
+      </c>
+      <c r="AB13" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC13" s="3">
+        <v>0</v>
+      </c>
+      <c r="AD13" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="AE13" s="19" t="s">
+      <c r="AE13" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="AF13" s="26" t="s">
+      <c r="AF13" s="8" t="s">
         <v>29</v>
       </c>
       <c r="AG13" s="1" t="s">
@@ -2312,7 +2301,7 @@
       <c r="AQ13">
         <v>0</v>
       </c>
-      <c r="AR13" s="10">
+      <c r="AR13" s="7">
         <v>1</v>
       </c>
       <c r="AS13" t="s">
@@ -2320,7 +2309,7 @@
       </c>
     </row>
     <row r="14" spans="1:46" x14ac:dyDescent="0.3">
-      <c r="A14" s="13">
+      <c r="A14">
         <v>0</v>
       </c>
       <c r="B14" s="4">
@@ -2371,52 +2360,52 @@
       <c r="Q14" s="4">
         <v>1</v>
       </c>
-      <c r="R14" s="6">
-        <v>1</v>
-      </c>
-      <c r="S14" s="17">
-        <v>0</v>
-      </c>
-      <c r="T14" s="14">
-        <v>0</v>
-      </c>
-      <c r="U14" s="14">
-        <v>0</v>
-      </c>
-      <c r="V14" s="14">
-        <v>0</v>
-      </c>
-      <c r="W14" s="14">
-        <v>1</v>
-      </c>
-      <c r="X14" s="14">
-        <v>0</v>
-      </c>
-      <c r="Y14" s="14">
-        <v>0</v>
-      </c>
-      <c r="Z14" s="14">
-        <v>0</v>
-      </c>
-      <c r="AA14" s="14">
-        <v>0</v>
-      </c>
-      <c r="AB14" s="14">
-        <v>0</v>
-      </c>
-      <c r="AC14" s="14">
-        <v>0</v>
-      </c>
-      <c r="AD14" s="14">
-        <v>0</v>
-      </c>
-      <c r="AE14" s="14">
-        <v>0</v>
-      </c>
-      <c r="AF14" s="24">
-        <v>0</v>
-      </c>
-      <c r="AG14" s="7" t="s">
+      <c r="R14" s="4">
+        <v>1</v>
+      </c>
+      <c r="S14" s="12">
+        <v>0</v>
+      </c>
+      <c r="T14" s="2">
+        <v>0</v>
+      </c>
+      <c r="U14" s="2">
+        <v>0</v>
+      </c>
+      <c r="V14" s="2">
+        <v>0</v>
+      </c>
+      <c r="W14" s="2">
+        <v>1</v>
+      </c>
+      <c r="X14" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y14" s="2">
+        <v>0</v>
+      </c>
+      <c r="Z14" s="2">
+        <v>0</v>
+      </c>
+      <c r="AA14" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB14" s="2">
+        <v>0</v>
+      </c>
+      <c r="AC14" s="2">
+        <v>0</v>
+      </c>
+      <c r="AD14" s="2">
+        <v>0</v>
+      </c>
+      <c r="AE14" s="2">
+        <v>0</v>
+      </c>
+      <c r="AF14" s="17">
+        <v>0</v>
+      </c>
+      <c r="AG14" s="4" t="s">
         <v>66</v>
       </c>
       <c r="AH14" s="2" t="s">
@@ -2446,7 +2435,7 @@
       <c r="AQ14">
         <v>0</v>
       </c>
-      <c r="AR14" s="10">
+      <c r="AR14" s="7">
         <v>1</v>
       </c>
       <c r="AS14" t="s">
@@ -2454,7 +2443,7 @@
       </c>
     </row>
     <row r="15" spans="1:46" x14ac:dyDescent="0.3">
-      <c r="A15" s="13">
+      <c r="A15">
         <v>0</v>
       </c>
       <c r="B15" s="4">
@@ -2505,52 +2494,52 @@
       <c r="Q15" s="4">
         <v>1</v>
       </c>
-      <c r="R15" s="12">
-        <v>1</v>
-      </c>
-      <c r="S15" s="18">
-        <v>0</v>
-      </c>
-      <c r="T15" s="14">
-        <v>1</v>
-      </c>
-      <c r="U15" s="14">
-        <v>0</v>
-      </c>
-      <c r="V15" s="14">
-        <v>0</v>
-      </c>
-      <c r="W15" s="14">
-        <v>0</v>
-      </c>
-      <c r="X15" s="14">
-        <v>0</v>
-      </c>
-      <c r="Y15" s="14">
-        <v>0</v>
-      </c>
-      <c r="Z15" s="14">
-        <v>0</v>
-      </c>
-      <c r="AA15" s="14">
-        <v>0</v>
-      </c>
-      <c r="AB15" s="14">
-        <v>0</v>
-      </c>
-      <c r="AC15" s="14">
-        <v>0</v>
-      </c>
-      <c r="AD15" s="14">
-        <v>0</v>
-      </c>
-      <c r="AE15" s="14">
-        <v>0</v>
-      </c>
-      <c r="AF15" s="24">
-        <v>0</v>
-      </c>
-      <c r="AG15" s="7" t="s">
+      <c r="R15" s="9">
+        <v>1</v>
+      </c>
+      <c r="S15" s="13">
+        <v>0</v>
+      </c>
+      <c r="T15" s="2">
+        <v>1</v>
+      </c>
+      <c r="U15" s="2">
+        <v>0</v>
+      </c>
+      <c r="V15" s="2">
+        <v>0</v>
+      </c>
+      <c r="W15" s="2">
+        <v>0</v>
+      </c>
+      <c r="X15" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y15" s="2">
+        <v>0</v>
+      </c>
+      <c r="Z15" s="2">
+        <v>0</v>
+      </c>
+      <c r="AA15" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB15" s="2">
+        <v>0</v>
+      </c>
+      <c r="AC15" s="2">
+        <v>0</v>
+      </c>
+      <c r="AD15" s="2">
+        <v>0</v>
+      </c>
+      <c r="AE15" s="2">
+        <v>0</v>
+      </c>
+      <c r="AF15" s="17">
+        <v>0</v>
+      </c>
+      <c r="AG15" s="4" t="s">
         <v>67</v>
       </c>
       <c r="AH15" s="2"/>
@@ -2578,7 +2567,7 @@
       <c r="AQ15">
         <v>1</v>
       </c>
-      <c r="AR15" s="10">
+      <c r="AR15" s="7">
         <v>0</v>
       </c>
       <c r="AS15" t="s">
@@ -2586,7 +2575,7 @@
       </c>
     </row>
     <row r="16" spans="1:46" x14ac:dyDescent="0.3">
-      <c r="A16" s="36">
+      <c r="A16" s="25">
         <v>0</v>
       </c>
       <c r="B16" s="3">
@@ -2637,49 +2626,49 @@
       <c r="Q16" s="3">
         <v>0</v>
       </c>
-      <c r="R16" s="26">
-        <v>1</v>
-      </c>
-      <c r="S16" s="35" t="s">
+      <c r="R16" s="8">
+        <v>1</v>
+      </c>
+      <c r="S16" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="T16" s="19">
-        <v>0</v>
-      </c>
-      <c r="U16" s="19" t="s">
+      <c r="T16" s="3">
+        <v>0</v>
+      </c>
+      <c r="U16" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="V16" s="19" t="s">
+      <c r="V16" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="W16" s="19">
-        <v>0</v>
-      </c>
-      <c r="X16" s="19" t="s">
+      <c r="W16" s="3">
+        <v>0</v>
+      </c>
+      <c r="X16" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="Y16" s="19" t="s">
+      <c r="Y16" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="Z16" s="19" t="s">
+      <c r="Z16" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="AA16" s="19">
-        <v>1</v>
-      </c>
-      <c r="AB16" s="19">
-        <v>0</v>
-      </c>
-      <c r="AC16" s="19">
-        <v>0</v>
-      </c>
-      <c r="AD16" s="19" t="s">
+      <c r="AA16" s="3">
+        <v>1</v>
+      </c>
+      <c r="AB16" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC16" s="3">
+        <v>0</v>
+      </c>
+      <c r="AD16" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="AE16" s="19" t="s">
+      <c r="AE16" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="AF16" s="26" t="s">
+      <c r="AF16" s="8" t="s">
         <v>29</v>
       </c>
       <c r="AG16" s="1" t="s">
@@ -2710,114 +2699,114 @@
       <c r="AQ16">
         <v>1</v>
       </c>
-      <c r="AR16" s="10">
+      <c r="AR16" s="7">
         <v>0</v>
       </c>
       <c r="AS16" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="17" spans="1:50" x14ac:dyDescent="0.3">
-      <c r="A17" s="9">
-        <v>0</v>
-      </c>
-      <c r="B17" s="21">
-        <v>0</v>
-      </c>
-      <c r="C17" s="21">
-        <v>0</v>
-      </c>
-      <c r="D17" s="21">
-        <v>0</v>
-      </c>
-      <c r="E17" s="21">
-        <v>0</v>
-      </c>
-      <c r="F17" s="21">
-        <v>0</v>
-      </c>
-      <c r="G17" s="21">
-        <v>0</v>
-      </c>
-      <c r="H17" s="21">
-        <v>0</v>
-      </c>
-      <c r="I17" s="21">
-        <v>0</v>
-      </c>
-      <c r="J17" s="21">
-        <v>0</v>
-      </c>
-      <c r="K17" s="21">
-        <v>0</v>
-      </c>
-      <c r="L17" s="21">
-        <v>0</v>
-      </c>
-      <c r="M17" s="21">
-        <v>0</v>
-      </c>
-      <c r="N17" s="21">
-        <v>0</v>
-      </c>
-      <c r="O17" s="21">
-        <v>0</v>
-      </c>
-      <c r="P17" s="21">
-        <v>0</v>
-      </c>
-      <c r="Q17" s="21">
-        <v>0</v>
-      </c>
-      <c r="R17" s="22">
-        <v>0</v>
-      </c>
-      <c r="S17" s="21">
-        <v>0</v>
-      </c>
-      <c r="T17" s="21">
-        <v>0</v>
-      </c>
-      <c r="U17" s="21">
-        <v>0</v>
-      </c>
-      <c r="V17" s="21">
-        <v>0</v>
-      </c>
-      <c r="W17" s="21">
-        <v>0</v>
-      </c>
-      <c r="X17" s="21">
-        <v>0</v>
-      </c>
-      <c r="Y17" s="21">
-        <v>0</v>
-      </c>
-      <c r="Z17" s="21">
-        <v>0</v>
-      </c>
-      <c r="AA17" s="21">
-        <v>1</v>
-      </c>
-      <c r="AB17" s="21">
-        <v>0</v>
-      </c>
-      <c r="AC17" s="21">
-        <v>0</v>
-      </c>
-      <c r="AD17" s="21">
-        <v>0</v>
-      </c>
-      <c r="AE17" s="21">
-        <v>0</v>
-      </c>
-      <c r="AF17" s="22">
-        <v>0</v>
-      </c>
-      <c r="AG17" s="20" t="s">
+    <row r="17" spans="1:45" x14ac:dyDescent="0.3">
+      <c r="A17" s="6">
+        <v>0</v>
+      </c>
+      <c r="B17" s="5">
+        <v>0</v>
+      </c>
+      <c r="C17" s="5">
+        <v>0</v>
+      </c>
+      <c r="D17" s="5">
+        <v>0</v>
+      </c>
+      <c r="E17" s="5">
+        <v>0</v>
+      </c>
+      <c r="F17" s="5">
+        <v>0</v>
+      </c>
+      <c r="G17" s="5">
+        <v>0</v>
+      </c>
+      <c r="H17" s="5">
+        <v>0</v>
+      </c>
+      <c r="I17" s="5">
+        <v>0</v>
+      </c>
+      <c r="J17" s="5">
+        <v>0</v>
+      </c>
+      <c r="K17" s="5">
+        <v>0</v>
+      </c>
+      <c r="L17" s="5">
+        <v>0</v>
+      </c>
+      <c r="M17" s="5">
+        <v>0</v>
+      </c>
+      <c r="N17" s="5">
+        <v>0</v>
+      </c>
+      <c r="O17" s="5">
+        <v>0</v>
+      </c>
+      <c r="P17" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q17" s="5">
+        <v>0</v>
+      </c>
+      <c r="R17" s="15">
+        <v>0</v>
+      </c>
+      <c r="S17" s="5">
+        <v>0</v>
+      </c>
+      <c r="T17" s="5">
+        <v>0</v>
+      </c>
+      <c r="U17" s="5">
+        <v>0</v>
+      </c>
+      <c r="V17" s="5">
+        <v>0</v>
+      </c>
+      <c r="W17" s="5">
+        <v>0</v>
+      </c>
+      <c r="X17" s="5">
+        <v>0</v>
+      </c>
+      <c r="Y17" s="5">
+        <v>0</v>
+      </c>
+      <c r="Z17" s="5">
+        <v>0</v>
+      </c>
+      <c r="AA17" s="5">
+        <v>1</v>
+      </c>
+      <c r="AB17" s="5">
+        <v>0</v>
+      </c>
+      <c r="AC17" s="5">
+        <v>0</v>
+      </c>
+      <c r="AD17" s="5">
+        <v>0</v>
+      </c>
+      <c r="AE17" s="5">
+        <v>0</v>
+      </c>
+      <c r="AF17" s="15">
+        <v>0</v>
+      </c>
+      <c r="AG17" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="AH17" s="9" t="s">
+      <c r="AH17" s="6" t="s">
         <v>34</v>
       </c>
       <c r="AJ17">
@@ -2844,114 +2833,114 @@
       <c r="AQ17">
         <v>1</v>
       </c>
-      <c r="AR17" s="10">
+      <c r="AR17" s="7">
         <v>1</v>
       </c>
       <c r="AS17" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="18" spans="1:50" x14ac:dyDescent="0.3">
-      <c r="A18" s="9">
-        <v>0</v>
-      </c>
-      <c r="B18" s="21">
-        <v>0</v>
-      </c>
-      <c r="C18" s="21">
-        <v>0</v>
-      </c>
-      <c r="D18" s="21">
-        <v>0</v>
-      </c>
-      <c r="E18" s="21">
-        <v>0</v>
-      </c>
-      <c r="F18" s="21">
-        <v>0</v>
-      </c>
-      <c r="G18" s="21">
-        <v>0</v>
-      </c>
-      <c r="H18" s="21">
-        <v>0</v>
-      </c>
-      <c r="I18" s="21">
-        <v>0</v>
-      </c>
-      <c r="J18" s="21">
-        <v>0</v>
-      </c>
-      <c r="K18" s="21">
-        <v>0</v>
-      </c>
-      <c r="L18" s="21">
-        <v>0</v>
-      </c>
-      <c r="M18" s="21">
-        <v>0</v>
-      </c>
-      <c r="N18" s="21">
-        <v>0</v>
-      </c>
-      <c r="O18" s="21">
-        <v>0</v>
-      </c>
-      <c r="P18" s="21">
-        <v>0</v>
-      </c>
-      <c r="Q18" s="21">
-        <v>0</v>
-      </c>
-      <c r="R18" s="22">
-        <v>0</v>
-      </c>
-      <c r="S18" s="21">
-        <v>0</v>
-      </c>
-      <c r="T18" s="21">
-        <v>0</v>
-      </c>
-      <c r="U18" s="21">
-        <v>0</v>
-      </c>
-      <c r="V18" s="21">
-        <v>0</v>
-      </c>
-      <c r="W18" s="21">
-        <v>0</v>
-      </c>
-      <c r="X18" s="21">
-        <v>0</v>
-      </c>
-      <c r="Y18" s="21">
-        <v>0</v>
-      </c>
-      <c r="Z18" s="21">
-        <v>0</v>
-      </c>
-      <c r="AA18" s="21">
-        <v>0</v>
-      </c>
-      <c r="AB18" s="21">
-        <v>1</v>
-      </c>
-      <c r="AC18" s="21">
-        <v>0</v>
-      </c>
-      <c r="AD18" s="21">
-        <v>0</v>
-      </c>
-      <c r="AE18" s="21">
-        <v>0</v>
-      </c>
-      <c r="AF18" s="22">
-        <v>0</v>
-      </c>
-      <c r="AG18" s="20" t="s">
+    <row r="18" spans="1:45" x14ac:dyDescent="0.3">
+      <c r="A18" s="6">
+        <v>0</v>
+      </c>
+      <c r="B18" s="5">
+        <v>0</v>
+      </c>
+      <c r="C18" s="5">
+        <v>0</v>
+      </c>
+      <c r="D18" s="5">
+        <v>0</v>
+      </c>
+      <c r="E18" s="5">
+        <v>0</v>
+      </c>
+      <c r="F18" s="5">
+        <v>0</v>
+      </c>
+      <c r="G18" s="5">
+        <v>0</v>
+      </c>
+      <c r="H18" s="5">
+        <v>0</v>
+      </c>
+      <c r="I18" s="5">
+        <v>0</v>
+      </c>
+      <c r="J18" s="5">
+        <v>0</v>
+      </c>
+      <c r="K18" s="5">
+        <v>0</v>
+      </c>
+      <c r="L18" s="5">
+        <v>0</v>
+      </c>
+      <c r="M18" s="5">
+        <v>0</v>
+      </c>
+      <c r="N18" s="5">
+        <v>0</v>
+      </c>
+      <c r="O18" s="5">
+        <v>0</v>
+      </c>
+      <c r="P18" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q18" s="5">
+        <v>0</v>
+      </c>
+      <c r="R18" s="15">
+        <v>0</v>
+      </c>
+      <c r="S18" s="5">
+        <v>0</v>
+      </c>
+      <c r="T18" s="5">
+        <v>0</v>
+      </c>
+      <c r="U18" s="5">
+        <v>0</v>
+      </c>
+      <c r="V18" s="5">
+        <v>0</v>
+      </c>
+      <c r="W18" s="5">
+        <v>0</v>
+      </c>
+      <c r="X18" s="5">
+        <v>0</v>
+      </c>
+      <c r="Y18" s="5">
+        <v>0</v>
+      </c>
+      <c r="Z18" s="5">
+        <v>0</v>
+      </c>
+      <c r="AA18" s="5">
+        <v>0</v>
+      </c>
+      <c r="AB18" s="5">
+        <v>1</v>
+      </c>
+      <c r="AC18" s="5">
+        <v>0</v>
+      </c>
+      <c r="AD18" s="5">
+        <v>0</v>
+      </c>
+      <c r="AE18" s="5">
+        <v>0</v>
+      </c>
+      <c r="AF18" s="15">
+        <v>0</v>
+      </c>
+      <c r="AG18" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="AH18" s="9" t="s">
+      <c r="AH18" s="6" t="s">
         <v>35</v>
       </c>
       <c r="AJ18">
@@ -2978,114 +2967,114 @@
       <c r="AQ18">
         <v>0</v>
       </c>
-      <c r="AR18" s="10">
+      <c r="AR18" s="7">
         <v>0</v>
       </c>
       <c r="AS18" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="19" spans="1:50" x14ac:dyDescent="0.3">
-      <c r="A19" s="9">
-        <v>0</v>
-      </c>
-      <c r="B19" s="21">
-        <v>0</v>
-      </c>
-      <c r="C19" s="21">
-        <v>0</v>
-      </c>
-      <c r="D19" s="21">
-        <v>0</v>
-      </c>
-      <c r="E19" s="21">
-        <v>0</v>
-      </c>
-      <c r="F19" s="21">
-        <v>0</v>
-      </c>
-      <c r="G19" s="21">
-        <v>0</v>
-      </c>
-      <c r="H19" s="21">
-        <v>0</v>
-      </c>
-      <c r="I19" s="21">
-        <v>0</v>
-      </c>
-      <c r="J19" s="21">
-        <v>0</v>
-      </c>
-      <c r="K19" s="21">
-        <v>0</v>
-      </c>
-      <c r="L19" s="21">
-        <v>0</v>
-      </c>
-      <c r="M19" s="21">
-        <v>0</v>
-      </c>
-      <c r="N19" s="21">
-        <v>0</v>
-      </c>
-      <c r="O19" s="21">
-        <v>0</v>
-      </c>
-      <c r="P19" s="21">
-        <v>0</v>
-      </c>
-      <c r="Q19" s="21">
-        <v>0</v>
-      </c>
-      <c r="R19" s="22">
-        <v>0</v>
-      </c>
-      <c r="S19" s="21">
-        <v>0</v>
-      </c>
-      <c r="T19" s="21">
-        <v>0</v>
-      </c>
-      <c r="U19" s="21">
-        <v>0</v>
-      </c>
-      <c r="V19" s="21">
-        <v>0</v>
-      </c>
-      <c r="W19" s="21">
-        <v>0</v>
-      </c>
-      <c r="X19" s="21">
-        <v>0</v>
-      </c>
-      <c r="Y19" s="21">
-        <v>0</v>
-      </c>
-      <c r="Z19" s="21">
-        <v>0</v>
-      </c>
-      <c r="AA19" s="21">
-        <v>0</v>
-      </c>
-      <c r="AB19" s="21">
-        <v>0</v>
-      </c>
-      <c r="AC19" s="21">
-        <v>1</v>
-      </c>
-      <c r="AD19" s="21">
-        <v>0</v>
-      </c>
-      <c r="AE19" s="21">
-        <v>0</v>
-      </c>
-      <c r="AF19" s="22">
-        <v>0</v>
-      </c>
-      <c r="AG19" s="20" t="s">
+    <row r="19" spans="1:45" x14ac:dyDescent="0.3">
+      <c r="A19" s="6">
+        <v>0</v>
+      </c>
+      <c r="B19" s="5">
+        <v>0</v>
+      </c>
+      <c r="C19" s="5">
+        <v>0</v>
+      </c>
+      <c r="D19" s="5">
+        <v>0</v>
+      </c>
+      <c r="E19" s="5">
+        <v>0</v>
+      </c>
+      <c r="F19" s="5">
+        <v>0</v>
+      </c>
+      <c r="G19" s="5">
+        <v>0</v>
+      </c>
+      <c r="H19" s="5">
+        <v>0</v>
+      </c>
+      <c r="I19" s="5">
+        <v>0</v>
+      </c>
+      <c r="J19" s="5">
+        <v>0</v>
+      </c>
+      <c r="K19" s="5">
+        <v>0</v>
+      </c>
+      <c r="L19" s="5">
+        <v>0</v>
+      </c>
+      <c r="M19" s="5">
+        <v>0</v>
+      </c>
+      <c r="N19" s="5">
+        <v>0</v>
+      </c>
+      <c r="O19" s="5">
+        <v>0</v>
+      </c>
+      <c r="P19" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q19" s="5">
+        <v>0</v>
+      </c>
+      <c r="R19" s="15">
+        <v>0</v>
+      </c>
+      <c r="S19" s="5">
+        <v>0</v>
+      </c>
+      <c r="T19" s="5">
+        <v>0</v>
+      </c>
+      <c r="U19" s="5">
+        <v>0</v>
+      </c>
+      <c r="V19" s="5">
+        <v>0</v>
+      </c>
+      <c r="W19" s="5">
+        <v>0</v>
+      </c>
+      <c r="X19" s="5">
+        <v>0</v>
+      </c>
+      <c r="Y19" s="5">
+        <v>0</v>
+      </c>
+      <c r="Z19" s="5">
+        <v>0</v>
+      </c>
+      <c r="AA19" s="5">
+        <v>0</v>
+      </c>
+      <c r="AB19" s="5">
+        <v>0</v>
+      </c>
+      <c r="AC19" s="5">
+        <v>1</v>
+      </c>
+      <c r="AD19" s="5">
+        <v>0</v>
+      </c>
+      <c r="AE19" s="5">
+        <v>0</v>
+      </c>
+      <c r="AF19" s="15">
+        <v>0</v>
+      </c>
+      <c r="AG19" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="AH19" s="9" t="s">
+      <c r="AH19" s="6" t="s">
         <v>36</v>
       </c>
       <c r="AJ19">
@@ -3112,114 +3101,114 @@
       <c r="AQ19">
         <v>0</v>
       </c>
-      <c r="AR19" s="10">
+      <c r="AR19" s="7">
         <v>0</v>
       </c>
       <c r="AS19" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="20" spans="1:50" x14ac:dyDescent="0.3">
-      <c r="A20" s="37">
-        <v>1</v>
-      </c>
-      <c r="B20" s="21">
-        <v>0</v>
-      </c>
-      <c r="C20" s="21">
-        <v>0</v>
-      </c>
-      <c r="D20" s="21" t="s">
+    <row r="20" spans="1:45" x14ac:dyDescent="0.3">
+      <c r="A20" s="6">
+        <v>1</v>
+      </c>
+      <c r="B20" s="5">
+        <v>0</v>
+      </c>
+      <c r="C20" s="5">
+        <v>0</v>
+      </c>
+      <c r="D20" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="E20" s="21" t="s">
+      <c r="E20" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="F20" s="21" t="s">
+      <c r="F20" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G20" s="21">
-        <v>0</v>
-      </c>
-      <c r="H20" s="21">
-        <v>0</v>
-      </c>
-      <c r="I20" s="21">
-        <v>0</v>
-      </c>
-      <c r="J20" s="21" t="s">
+      <c r="G20" s="5">
+        <v>0</v>
+      </c>
+      <c r="H20" s="5">
+        <v>0</v>
+      </c>
+      <c r="I20" s="5">
+        <v>0</v>
+      </c>
+      <c r="J20" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="K20" s="21" t="s">
+      <c r="K20" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="L20" s="21" t="s">
+      <c r="L20" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="M20" s="21" t="s">
+      <c r="M20" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="N20" s="21" t="s">
+      <c r="N20" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="O20" s="21" t="s">
+      <c r="O20" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="P20" s="21">
-        <v>0</v>
-      </c>
-      <c r="Q20" s="21">
-        <v>0</v>
-      </c>
-      <c r="R20" s="22">
-        <v>0</v>
-      </c>
-      <c r="S20" s="21">
-        <v>0</v>
-      </c>
-      <c r="T20" s="21">
-        <v>0</v>
-      </c>
-      <c r="U20" s="21">
-        <v>0</v>
-      </c>
-      <c r="V20" s="21">
-        <v>0</v>
-      </c>
-      <c r="W20" s="21">
-        <v>0</v>
-      </c>
-      <c r="X20" s="21">
-        <v>0</v>
-      </c>
-      <c r="Y20" s="21">
-        <v>0</v>
-      </c>
-      <c r="Z20" s="21">
-        <v>0</v>
-      </c>
-      <c r="AA20" s="21">
-        <v>0</v>
-      </c>
-      <c r="AB20" s="21">
-        <v>0</v>
-      </c>
-      <c r="AC20" s="21">
-        <v>0</v>
-      </c>
-      <c r="AD20" s="21">
-        <v>0</v>
-      </c>
-      <c r="AE20" s="21">
-        <v>0</v>
-      </c>
-      <c r="AF20" s="22">
-        <v>0</v>
-      </c>
-      <c r="AG20" s="20" t="s">
+      <c r="P20" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q20" s="5">
+        <v>0</v>
+      </c>
+      <c r="R20" s="15">
+        <v>0</v>
+      </c>
+      <c r="S20" s="5">
+        <v>0</v>
+      </c>
+      <c r="T20" s="5">
+        <v>0</v>
+      </c>
+      <c r="U20" s="5">
+        <v>0</v>
+      </c>
+      <c r="V20" s="5">
+        <v>0</v>
+      </c>
+      <c r="W20" s="5">
+        <v>0</v>
+      </c>
+      <c r="X20" s="5">
+        <v>0</v>
+      </c>
+      <c r="Y20" s="5">
+        <v>0</v>
+      </c>
+      <c r="Z20" s="5">
+        <v>0</v>
+      </c>
+      <c r="AA20" s="5">
+        <v>0</v>
+      </c>
+      <c r="AB20" s="5">
+        <v>0</v>
+      </c>
+      <c r="AC20" s="5">
+        <v>0</v>
+      </c>
+      <c r="AD20" s="5">
+        <v>0</v>
+      </c>
+      <c r="AE20" s="5">
+        <v>0</v>
+      </c>
+      <c r="AF20" s="15">
+        <v>0</v>
+      </c>
+      <c r="AG20" s="14" t="s">
         <v>75</v>
       </c>
-      <c r="AH20" s="37" t="s">
+      <c r="AH20" s="6" t="s">
         <v>76</v>
       </c>
       <c r="AJ20">
@@ -3246,15 +3235,14 @@
       <c r="AQ20">
         <v>0</v>
       </c>
-      <c r="AR20" s="10">
+      <c r="AR20" s="7">
         <v>1</v>
       </c>
       <c r="AS20" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="21" spans="1:50" x14ac:dyDescent="0.3">
-      <c r="R21" s="8"/>
+    <row r="21" spans="1:45" x14ac:dyDescent="0.3">
       <c r="AJ21">
         <v>0</v>
       </c>
@@ -3279,14 +3267,17 @@
       <c r="AQ21">
         <v>1</v>
       </c>
-      <c r="AR21" s="10">
+      <c r="AR21" s="7">
         <v>0</v>
       </c>
       <c r="AS21" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="22" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:45" x14ac:dyDescent="0.3">
+      <c r="D22" t="s">
+        <v>89</v>
+      </c>
       <c r="AJ22">
         <v>0</v>
       </c>
@@ -3311,14 +3302,14 @@
       <c r="AQ22">
         <v>1</v>
       </c>
-      <c r="AR22" s="10">
+      <c r="AR22" s="7">
         <v>1</v>
       </c>
       <c r="AS22" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="23" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:45" x14ac:dyDescent="0.3">
       <c r="AJ23">
         <v>0</v>
       </c>
@@ -3343,14 +3334,17 @@
       <c r="AQ23">
         <v>1</v>
       </c>
-      <c r="AR23" s="10">
+      <c r="AR23" s="7">
         <v>1</v>
       </c>
       <c r="AS23" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="24" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:45" x14ac:dyDescent="0.3">
+      <c r="J24" t="s">
+        <v>82</v>
+      </c>
       <c r="AJ24">
         <v>0</v>
       </c>
@@ -3375,14 +3369,17 @@
       <c r="AQ24">
         <v>1</v>
       </c>
-      <c r="AR24" s="10">
+      <c r="AR24" s="7">
         <v>1</v>
       </c>
       <c r="AS24" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="25" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:45" x14ac:dyDescent="0.3">
+      <c r="J25" t="s">
+        <v>83</v>
+      </c>
       <c r="AJ25">
         <v>0</v>
       </c>
@@ -3407,14 +3404,17 @@
       <c r="AQ25">
         <v>1</v>
       </c>
-      <c r="AR25" s="10">
-        <v>1</v>
-      </c>
-      <c r="AS25" s="13" t="s">
+      <c r="AR25" s="7">
+        <v>1</v>
+      </c>
+      <c r="AS25" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="26" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:45" x14ac:dyDescent="0.3">
+      <c r="J26" t="s">
+        <v>85</v>
+      </c>
       <c r="AJ26">
         <v>0</v>
       </c>
@@ -3439,14 +3439,17 @@
       <c r="AQ26">
         <v>1</v>
       </c>
-      <c r="AR26" s="10">
-        <v>1</v>
-      </c>
-      <c r="AS26" s="29">
+      <c r="AR26" s="7">
+        <v>1</v>
+      </c>
+      <c r="AS26" s="2">
         <v>-1</v>
       </c>
     </row>
-    <row r="27" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:45" x14ac:dyDescent="0.3">
+      <c r="J27" t="s">
+        <v>84</v>
+      </c>
       <c r="AJ27">
         <v>0</v>
       </c>
@@ -3471,14 +3474,17 @@
       <c r="AQ27">
         <v>1</v>
       </c>
-      <c r="AR27" s="10">
-        <v>1</v>
-      </c>
-      <c r="AS27" s="29">
+      <c r="AR27" s="7">
+        <v>1</v>
+      </c>
+      <c r="AS27" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:45" x14ac:dyDescent="0.3">
+      <c r="J28" t="s">
+        <v>87</v>
+      </c>
       <c r="AJ28">
         <v>0</v>
       </c>
@@ -3503,60 +3509,22 @@
       <c r="AQ28">
         <v>1</v>
       </c>
-      <c r="AR28" s="10">
-        <v>1</v>
-      </c>
-      <c r="AS28" s="29">
+      <c r="AR28" s="7">
+        <v>1</v>
+      </c>
+      <c r="AS28" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:50" x14ac:dyDescent="0.3">
-      <c r="AW29" s="8"/>
-      <c r="AX29" s="8"/>
+    <row r="29" spans="1:45" x14ac:dyDescent="0.3">
+      <c r="J29" t="s">
+        <v>86</v>
+      </c>
     </row>
-    <row r="30" spans="1:50" x14ac:dyDescent="0.3">
-      <c r="AW30" s="8"/>
-      <c r="AX30" s="8"/>
-    </row>
-    <row r="31" spans="1:50" x14ac:dyDescent="0.3">
-      <c r="AW31" s="8"/>
-      <c r="AX31" s="8"/>
-    </row>
-    <row r="32" spans="1:50" x14ac:dyDescent="0.3">
-      <c r="AW32" s="8"/>
-      <c r="AX32" s="8"/>
-    </row>
-    <row r="33" spans="22:50" x14ac:dyDescent="0.3">
-      <c r="AW33" s="8"/>
-      <c r="AX33" s="8"/>
-    </row>
-    <row r="34" spans="22:50" x14ac:dyDescent="0.3">
-      <c r="AW34" s="8"/>
-      <c r="AX34" s="8"/>
-    </row>
-    <row r="35" spans="22:50" x14ac:dyDescent="0.3">
-      <c r="AW35" s="8"/>
-      <c r="AX35" s="8"/>
-    </row>
-    <row r="36" spans="22:50" x14ac:dyDescent="0.3">
-      <c r="AW36" s="8"/>
-      <c r="AX36" s="8"/>
-    </row>
-    <row r="37" spans="22:50" x14ac:dyDescent="0.3">
-      <c r="AW37" s="8"/>
-      <c r="AX37" s="8"/>
-    </row>
-    <row r="38" spans="22:50" x14ac:dyDescent="0.3">
-      <c r="AW38" s="8"/>
-      <c r="AX38" s="8"/>
-    </row>
-    <row r="39" spans="22:50" x14ac:dyDescent="0.3">
-      <c r="AW39" s="8"/>
-      <c r="AX39" s="8"/>
-    </row>
-    <row r="40" spans="22:50" x14ac:dyDescent="0.3">
-      <c r="V40" s="8"/>
-      <c r="W40" s="8"/>
+    <row r="30" spans="1:45" x14ac:dyDescent="0.3">
+      <c r="J30" t="s">
+        <v>88</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>